<commit_message>
v5.3.1 Introducing company separation in transactions
</commit_message>
<xml_diff>
--- a/Flowchart.xlsx
+++ b/Flowchart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\eiad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfb20fd7996edf0d/Code/htdocs/eiad/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1021245D-8169-4A82-8A78-0F8EFE22FE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{49C059A5-764B-47C4-B6D8-E7CE13A22E0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49C059A5-764B-47C4-B6D8-E7CE13A22E0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +208,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,17 +470,17 @@
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="14.796875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -494,7 +494,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>3</v>
       </c>
@@ -505,7 +505,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -519,7 +519,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>3</v>
       </c>
@@ -530,7 +530,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -544,7 +544,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>3</v>
       </c>
@@ -555,7 +555,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -569,7 +569,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>3</v>
       </c>

</xml_diff>